<commit_message>
Create staged bar graph
- make a presentable version of the plot
- update summary excel files by adding additional column with symptom negative/positive (for later statistical assessment)
</commit_message>
<xml_diff>
--- a/MM20230516_summary_visual_score_cell_death.xlsx
+++ b/MM20230516_summary_visual_score_cell_death.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mende012\Documents\Bioinformatics\Cell_death\Analysis_disease_symptoms_visual_scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACEF773-F5CC-42A6-B3B1-3ED85E51AF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8602F302-3719-4AD1-8CBD-10A88CFE5A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4A0879DF-965F-48AF-852A-00BCE3CACC5D}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7360" xr2:uid="{4A0879DF-965F-48AF-852A-00BCE3CACC5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data" sheetId="1" r:id="rId1"/>
@@ -370,13 +370,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1844,8 +1844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C77FE1-827D-48C6-93F5-1E0B6AC7653F}">
   <dimension ref="A1:AE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1854,7 +1854,7 @@
     <col min="3" max="3" width="11.08984375" customWidth="1"/>
     <col min="4" max="4" width="13.36328125" customWidth="1"/>
     <col min="9" max="9" width="12.1796875" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" style="12" customWidth="1"/>
     <col min="11" max="14" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
@@ -1886,7 +1886,7 @@
       <c r="I1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>71</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -1948,7 +1948,7 @@
         <f>SUM(D3:H3)</f>
         <v>10</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <f>((D3*$D$2)+(E3*$E$2)+(F3*$F$2)+(G3*$G$2)+(H3*$H$2))/I3</f>
         <v>0</v>
       </c>
@@ -1990,7 +1990,7 @@
         <f>SUM(D4:H4)</f>
         <v>10</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
         <f>((D4*$D$2)+(E4*$E$2)+(F4*$F$2)+(G4*$G$2)+(H4*$H$2))/I4</f>
         <v>4</v>
       </c>
@@ -2032,8 +2032,8 @@
         <f t="shared" ref="I5:I43" si="0">SUM(D5:H5)</f>
         <v>10</v>
       </c>
-      <c r="J5" s="13">
-        <f t="shared" ref="J4:J43" si="1">((D5*$D$2)+(E5*$E$2)+(F5*$F$2)+(G5*$G$2)+(H5*$H$2))/I5</f>
+      <c r="J5" s="12">
+        <f t="shared" ref="J5:J43" si="1">((D5*$D$2)+(E5*$E$2)+(F5*$F$2)+(G5*$G$2)+(H5*$H$2))/I5</f>
         <v>0</v>
       </c>
       <c r="O5" s="4">
@@ -2074,7 +2074,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2116,7 +2116,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2154,7 +2154,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="12">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -2192,7 +2192,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2232,7 +2232,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="12">
         <f t="shared" si="1"/>
         <v>9.0909090909090912E-2</v>
       </c>
@@ -2271,7 +2271,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="12">
         <f t="shared" si="1"/>
         <v>0.27272727272727271</v>
       </c>
@@ -2310,7 +2310,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="12">
         <f t="shared" si="1"/>
         <v>3.1818181818181817</v>
       </c>
@@ -2349,7 +2349,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2389,7 +2389,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="12">
         <f t="shared" si="1"/>
         <v>3.9047619047619047</v>
       </c>
@@ -2429,7 +2429,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="12">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -2465,7 +2465,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="12">
         <f t="shared" si="1"/>
         <v>9.0909090909090912E-2</v>
       </c>
@@ -2501,7 +2501,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="12">
         <f t="shared" si="1"/>
         <v>2.7</v>
       </c>
@@ -2537,7 +2537,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="12">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
@@ -2573,7 +2573,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2610,7 +2610,7 @@
         <f>SUM(D20:H20)</f>
         <v>20</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="12">
         <f t="shared" si="1"/>
         <v>3.2</v>
       </c>
@@ -2647,7 +2647,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2683,7 +2683,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2719,7 +2719,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="12">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
@@ -2753,7 +2753,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2786,7 +2786,7 @@
       <c r="I25" s="6">
         <v>51</v>
       </c>
-      <c r="J25" s="13">
+      <c r="J25" s="12">
         <f t="shared" si="1"/>
         <v>0.47058823529411764</v>
       </c>
@@ -2842,7 +2842,7 @@
       <c r="I26" s="6">
         <v>51</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="12">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" s="9">
         <v>1</v>
@@ -2892,11 +2892,11 @@
       </c>
       <c r="I27" s="6">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J27" s="13">
+        <v>9</v>
+      </c>
+      <c r="J27" s="12">
         <f t="shared" si="1"/>
-        <v>0.3</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
@@ -2928,7 +2928,7 @@
         <v>53</v>
       </c>
       <c r="D28" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E28" s="9">
         <v>0</v>
@@ -2944,11 +2944,11 @@
       </c>
       <c r="I28" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J28" s="13">
+        <v>9</v>
+      </c>
+      <c r="J28" s="12">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -2998,7 +2998,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="12">
         <f t="shared" si="1"/>
         <v>2.375</v>
       </c>
@@ -3050,7 +3050,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="12">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
@@ -3102,7 +3102,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3154,7 +3154,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J32" s="13">
+      <c r="J32" s="12">
         <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
@@ -3206,7 +3206,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J33" s="13">
+      <c r="J33" s="12">
         <f t="shared" si="1"/>
         <v>2.6666666666666665</v>
       </c>
@@ -3258,7 +3258,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="12">
         <f t="shared" si="1"/>
         <v>0.22222222222222221</v>
       </c>
@@ -3313,7 +3313,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J35" s="13">
+      <c r="J35" s="12">
         <f t="shared" si="1"/>
         <v>1.4444444444444444</v>
       </c>
@@ -3365,7 +3365,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="12">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -3420,7 +3420,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J37" s="13">
+      <c r="J37" s="12">
         <f t="shared" si="1"/>
         <v>2.6666666666666665</v>
       </c>
@@ -3472,7 +3472,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="12">
         <f t="shared" si="1"/>
         <v>1.5555555555555556</v>
       </c>
@@ -3524,7 +3524,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J39" s="13">
+      <c r="J39" s="12">
         <f t="shared" si="1"/>
         <v>0.90909090909090906</v>
       </c>
@@ -3576,7 +3576,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J40" s="13">
+      <c r="J40" s="12">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
@@ -3631,7 +3631,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J41" s="13">
+      <c r="J41" s="12">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -3665,7 +3665,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J42" s="13">
+      <c r="J42" s="12">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
@@ -3699,7 +3699,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J43" s="13">
+      <c r="J43" s="12">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
@@ -3756,13 +3756,13 @@
         <f>'Raw data'!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">

</xml_diff>